<commit_message>
Add business account to assessment summary
</commit_message>
<xml_diff>
--- a/platform/src/main/resources/jxls/assessments_summary_template.xlsx
+++ b/platform/src/main/resources/jxls/assessments_summary_template.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3560C534-EDA1-48E0-A144-24C6B0F67ABF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E11E9DF7-BC3A-4647-9C86-61B12E779851}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-jx:area(lastCell="G6")</t>
+jx:area(lastCell="H6")</t>
         </r>
       </text>
     </comment>
@@ -65,7 +65,7 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-jx:each(items="assessments" var="a" lastCell="G6" orderBy="displayName")</t>
+jx:each(items="assessments" var="a" lastCell="H6" orderBy="displayName")</t>
         </r>
       </text>
     </comment>
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>${exportedAt}</t>
   </si>
@@ -131,6 +131,12 @@
   </si>
   <si>
     <t>Выгрузка сводной информации по ассессментам сотрудников компании</t>
+  </si>
+  <si>
+    <t>Бизнес аккаунт</t>
+  </si>
+  <si>
+    <t>${a.ba.name}</t>
   </si>
 </sst>
 </file>
@@ -232,7 +238,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -241,20 +247,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color indexed="64"/>
       </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
       <bottom style="thin">
-        <color theme="4"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -263,10 +266,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -274,10 +275,6 @@
     <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -288,13 +285,24 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -302,7 +310,7 @@
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
     <cellStyle name="Финансовый" xfId="1" builtinId="3"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="9">
     <dxf>
       <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
       <fill>
@@ -312,6 +320,24 @@
         </patternFill>
       </fill>
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
     </dxf>
     <dxf>
       <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
@@ -322,15 +348,134 @@
         </patternFill>
       </fill>
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
     </dxf>
     <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
     </dxf>
     <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
     </dxf>
     <dxf>
       <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
     </dxf>
     <dxf>
       <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
@@ -341,6 +486,46 @@
         </patternFill>
       </fill>
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -366,6 +551,22 @@
           <bgColor rgb="FFE84C05"/>
         </patternFill>
       </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -429,12 +630,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Таблица1" displayName="Таблица1" ref="A5:G6" totalsRowShown="0" headerRowDxfId="6">
-  <autoFilter ref="A5:G6" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Сотрудник"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Дата устройства" dataDxfId="5"/>
-    <tableColumn id="9" xr3:uid="{885B8CA8-00F0-44ED-A856-0BC674D65CF7}" name="Дней без ассессмента" dataDxfId="4" dataCellStyle="Финансовый"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Таблица1" displayName="Таблица1" ref="A5:H6" totalsRowShown="0" headerRowDxfId="8">
+  <autoFilter ref="A5:H6" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Сотрудник" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Дата устройства" dataDxfId="6"/>
+    <tableColumn id="9" xr3:uid="{885B8CA8-00F0-44ED-A856-0BC674D65CF7}" name="Дней без ассессмента" dataDxfId="5" dataCellStyle="Финансовый"/>
+    <tableColumn id="2" xr3:uid="{800FC796-5D37-4D0A-9235-21DD7EDDFFC6}" name="Бизнес аккаунт" dataDxfId="4" dataCellStyle="Финансовый"/>
     <tableColumn id="8" xr3:uid="{F4397C7A-0AA8-4E96-B612-0BC651C56D20}" name="Название" dataDxfId="3"/>
     <tableColumn id="7" xr3:uid="{3D8A3B5D-81B9-40E1-8FE8-15F0B8DA312B}" name="Роль" dataDxfId="2"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Запланирован" dataDxfId="1"/>
@@ -765,10 +967,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -776,110 +978,119 @@
     <col min="1" max="1" width="41.59765625" customWidth="1"/>
     <col min="2" max="2" width="18.3984375" customWidth="1"/>
     <col min="3" max="3" width="21.53125" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="21.53125" customWidth="1"/>
-    <col min="6" max="6" width="20.1328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="28.796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="21.53125" customWidth="1"/>
+    <col min="7" max="7" width="20.1328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28.796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="30.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="3"/>
-      <c r="B1" s="12" t="s">
+    <row r="1" spans="1:8" ht="30.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="1"/>
+      <c r="B1" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A2" s="4"/>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="9"/>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A2" s="2"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="5"/>
     </row>
-    <row r="3" spans="1:7" ht="10.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="4"/>
-      <c r="B3" s="10" t="s">
+    <row r="3" spans="1:8" ht="10.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A3" s="2"/>
+      <c r="B3" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="17"/>
     </row>
-    <row r="4" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A4" s="6"/>
-      <c r="B4" s="11"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11" t="s">
+    <row r="4" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A4" s="7"/>
+      <c r="B4" s="13"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11" t="s">
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="11"/>
+      <c r="H4" s="14"/>
     </row>
-    <row r="5" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A5" s="2" t="s">
+    <row r="5" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A5" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="F5" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="G5" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="H5" s="8" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A6" t="s">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A6" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="F6" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="G6" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="G6" s="5" t="s">
+      <c r="H6" s="10" t="s">
         <v>7</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="B1:G1"/>
-    <mergeCell ref="F3:G3"/>
+  <mergeCells count="4">
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="D4:F4"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>